<commit_message>
For Excel implementation, added color-coding based on species, as well as opacity/transparency
</commit_message>
<xml_diff>
--- a/all_visualizations/kf_excel_penglings.csv.xlsx
+++ b/all_visualizations/kf_excel_penglings.csv.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klaud\WebstormProjects\klaudio-fusha-a2-datavis-5ways\a2-DataVis-5ways\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klaud\WebstormProjects\klaudio-fusha-a2-datavis-5ways\a2-DataVis-5ways\all_visualizations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37CE8A2-EE7B-4664-A9D0-EB48EF3088AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4112ED8-012D-410A-AF1A-ACBACD74EC77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{298BFD60-299E-47A5-8AF2-E192D2EEC218}"/>
   </bookViews>
@@ -606,6 +606,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF21C1A6"/>
+      <color rgb="FFD256C3"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -641,18 +647,10 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>kf_excel_penglings!$G$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>body_mass_g</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Adelie</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="38100" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -663,22 +661,22 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2">
+                  <a:alpha val="70000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>kf_excel_penglings!$F$2:$F$345</c:f>
+              <c:f>kf_excel_penglings!$F$2:$F$153</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="342"/>
+                <c:ptCount val="151"/>
                 <c:pt idx="0">
                   <c:v>181</c:v>
                 </c:pt>
@@ -1131,589 +1129,16 @@
                 </c:pt>
                 <c:pt idx="150">
                   <c:v>201</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>211</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>230</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>218</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>215</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>211</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>219</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>209</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>215</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>214</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>216</c:v>
-                </c:pt>
-                <c:pt idx="163">
-                  <c:v>214</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>213</c:v>
-                </c:pt>
-                <c:pt idx="165">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="166">
-                  <c:v>217</c:v>
-                </c:pt>
-                <c:pt idx="167">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="168">
-                  <c:v>221</c:v>
-                </c:pt>
-                <c:pt idx="169">
-                  <c:v>209</c:v>
-                </c:pt>
-                <c:pt idx="170">
-                  <c:v>222</c:v>
-                </c:pt>
-                <c:pt idx="171">
-                  <c:v>218</c:v>
-                </c:pt>
-                <c:pt idx="172">
-                  <c:v>215</c:v>
-                </c:pt>
-                <c:pt idx="173">
-                  <c:v>213</c:v>
-                </c:pt>
-                <c:pt idx="174">
-                  <c:v>215</c:v>
-                </c:pt>
-                <c:pt idx="175">
-                  <c:v>215</c:v>
-                </c:pt>
-                <c:pt idx="176">
-                  <c:v>215</c:v>
-                </c:pt>
-                <c:pt idx="177">
-                  <c:v>216</c:v>
-                </c:pt>
-                <c:pt idx="178">
-                  <c:v>215</c:v>
-                </c:pt>
-                <c:pt idx="179">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="180">
-                  <c:v>220</c:v>
-                </c:pt>
-                <c:pt idx="181">
-                  <c:v>222</c:v>
-                </c:pt>
-                <c:pt idx="182">
-                  <c:v>209</c:v>
-                </c:pt>
-                <c:pt idx="183">
-                  <c:v>207</c:v>
-                </c:pt>
-                <c:pt idx="184">
-                  <c:v>230</c:v>
-                </c:pt>
-                <c:pt idx="185">
-                  <c:v>220</c:v>
-                </c:pt>
-                <c:pt idx="186">
-                  <c:v>220</c:v>
-                </c:pt>
-                <c:pt idx="187">
-                  <c:v>213</c:v>
-                </c:pt>
-                <c:pt idx="188">
-                  <c:v>219</c:v>
-                </c:pt>
-                <c:pt idx="189">
-                  <c:v>208</c:v>
-                </c:pt>
-                <c:pt idx="190">
-                  <c:v>208</c:v>
-                </c:pt>
-                <c:pt idx="191">
-                  <c:v>208</c:v>
-                </c:pt>
-                <c:pt idx="192">
-                  <c:v>225</c:v>
-                </c:pt>
-                <c:pt idx="193">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="194">
-                  <c:v>216</c:v>
-                </c:pt>
-                <c:pt idx="195">
-                  <c:v>222</c:v>
-                </c:pt>
-                <c:pt idx="196">
-                  <c:v>217</c:v>
-                </c:pt>
-                <c:pt idx="197">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="198">
-                  <c:v>225</c:v>
-                </c:pt>
-                <c:pt idx="199">
-                  <c:v>213</c:v>
-                </c:pt>
-                <c:pt idx="200">
-                  <c:v>215</c:v>
-                </c:pt>
-                <c:pt idx="201">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="202">
-                  <c:v>220</c:v>
-                </c:pt>
-                <c:pt idx="203">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="204">
-                  <c:v>225</c:v>
-                </c:pt>
-                <c:pt idx="205">
-                  <c:v>217</c:v>
-                </c:pt>
-                <c:pt idx="206">
-                  <c:v>220</c:v>
-                </c:pt>
-                <c:pt idx="207">
-                  <c:v>208</c:v>
-                </c:pt>
-                <c:pt idx="208">
-                  <c:v>220</c:v>
-                </c:pt>
-                <c:pt idx="209">
-                  <c:v>208</c:v>
-                </c:pt>
-                <c:pt idx="210">
-                  <c:v>224</c:v>
-                </c:pt>
-                <c:pt idx="211">
-                  <c:v>208</c:v>
-                </c:pt>
-                <c:pt idx="212">
-                  <c:v>221</c:v>
-                </c:pt>
-                <c:pt idx="213">
-                  <c:v>214</c:v>
-                </c:pt>
-                <c:pt idx="214">
-                  <c:v>231</c:v>
-                </c:pt>
-                <c:pt idx="215">
-                  <c:v>219</c:v>
-                </c:pt>
-                <c:pt idx="216">
-                  <c:v>230</c:v>
-                </c:pt>
-                <c:pt idx="217">
-                  <c:v>214</c:v>
-                </c:pt>
-                <c:pt idx="218">
-                  <c:v>229</c:v>
-                </c:pt>
-                <c:pt idx="219">
-                  <c:v>220</c:v>
-                </c:pt>
-                <c:pt idx="220">
-                  <c:v>223</c:v>
-                </c:pt>
-                <c:pt idx="221">
-                  <c:v>216</c:v>
-                </c:pt>
-                <c:pt idx="222">
-                  <c:v>221</c:v>
-                </c:pt>
-                <c:pt idx="223">
-                  <c:v>221</c:v>
-                </c:pt>
-                <c:pt idx="224">
-                  <c:v>217</c:v>
-                </c:pt>
-                <c:pt idx="225">
-                  <c:v>216</c:v>
-                </c:pt>
-                <c:pt idx="226">
-                  <c:v>230</c:v>
-                </c:pt>
-                <c:pt idx="227">
-                  <c:v>209</c:v>
-                </c:pt>
-                <c:pt idx="228">
-                  <c:v>220</c:v>
-                </c:pt>
-                <c:pt idx="229">
-                  <c:v>215</c:v>
-                </c:pt>
-                <c:pt idx="230">
-                  <c:v>223</c:v>
-                </c:pt>
-                <c:pt idx="231">
-                  <c:v>212</c:v>
-                </c:pt>
-                <c:pt idx="232">
-                  <c:v>221</c:v>
-                </c:pt>
-                <c:pt idx="233">
-                  <c:v>212</c:v>
-                </c:pt>
-                <c:pt idx="234">
-                  <c:v>224</c:v>
-                </c:pt>
-                <c:pt idx="235">
-                  <c:v>212</c:v>
-                </c:pt>
-                <c:pt idx="236">
-                  <c:v>228</c:v>
-                </c:pt>
-                <c:pt idx="237">
-                  <c:v>218</c:v>
-                </c:pt>
-                <c:pt idx="238">
-                  <c:v>218</c:v>
-                </c:pt>
-                <c:pt idx="239">
-                  <c:v>212</c:v>
-                </c:pt>
-                <c:pt idx="240">
-                  <c:v>230</c:v>
-                </c:pt>
-                <c:pt idx="241">
-                  <c:v>218</c:v>
-                </c:pt>
-                <c:pt idx="242">
-                  <c:v>228</c:v>
-                </c:pt>
-                <c:pt idx="243">
-                  <c:v>212</c:v>
-                </c:pt>
-                <c:pt idx="244">
-                  <c:v>224</c:v>
-                </c:pt>
-                <c:pt idx="245">
-                  <c:v>214</c:v>
-                </c:pt>
-                <c:pt idx="246">
-                  <c:v>226</c:v>
-                </c:pt>
-                <c:pt idx="247">
-                  <c:v>216</c:v>
-                </c:pt>
-                <c:pt idx="248">
-                  <c:v>222</c:v>
-                </c:pt>
-                <c:pt idx="249">
-                  <c:v>203</c:v>
-                </c:pt>
-                <c:pt idx="250">
-                  <c:v>225</c:v>
-                </c:pt>
-                <c:pt idx="251">
-                  <c:v>219</c:v>
-                </c:pt>
-                <c:pt idx="252">
-                  <c:v>228</c:v>
-                </c:pt>
-                <c:pt idx="253">
-                  <c:v>215</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v>228</c:v>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v>216</c:v>
-                </c:pt>
-                <c:pt idx="256">
-                  <c:v>215</c:v>
-                </c:pt>
-                <c:pt idx="257">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="258">
-                  <c:v>219</c:v>
-                </c:pt>
-                <c:pt idx="259">
-                  <c:v>208</c:v>
-                </c:pt>
-                <c:pt idx="260">
-                  <c:v>209</c:v>
-                </c:pt>
-                <c:pt idx="261">
-                  <c:v>216</c:v>
-                </c:pt>
-                <c:pt idx="262">
-                  <c:v>229</c:v>
-                </c:pt>
-                <c:pt idx="263">
-                  <c:v>213</c:v>
-                </c:pt>
-                <c:pt idx="264">
-                  <c:v>230</c:v>
-                </c:pt>
-                <c:pt idx="265">
-                  <c:v>217</c:v>
-                </c:pt>
-                <c:pt idx="266">
-                  <c:v>230</c:v>
-                </c:pt>
-                <c:pt idx="267">
-                  <c:v>217</c:v>
-                </c:pt>
-                <c:pt idx="268">
-                  <c:v>222</c:v>
-                </c:pt>
-                <c:pt idx="269">
-                  <c:v>214</c:v>
-                </c:pt>
-                <c:pt idx="270">
-                  <c:v>215</c:v>
-                </c:pt>
-                <c:pt idx="271">
-                  <c:v>222</c:v>
-                </c:pt>
-                <c:pt idx="272">
-                  <c:v>212</c:v>
-                </c:pt>
-                <c:pt idx="273">
-                  <c:v>213</c:v>
-                </c:pt>
-                <c:pt idx="274">
-                  <c:v>192</c:v>
-                </c:pt>
-                <c:pt idx="275">
-                  <c:v>196</c:v>
-                </c:pt>
-                <c:pt idx="276">
-                  <c:v>193</c:v>
-                </c:pt>
-                <c:pt idx="277">
-                  <c:v>188</c:v>
-                </c:pt>
-                <c:pt idx="278">
-                  <c:v>197</c:v>
-                </c:pt>
-                <c:pt idx="279">
-                  <c:v>198</c:v>
-                </c:pt>
-                <c:pt idx="280">
-                  <c:v>178</c:v>
-                </c:pt>
-                <c:pt idx="281">
-                  <c:v>197</c:v>
-                </c:pt>
-                <c:pt idx="282">
-                  <c:v>195</c:v>
-                </c:pt>
-                <c:pt idx="283">
-                  <c:v>198</c:v>
-                </c:pt>
-                <c:pt idx="284">
-                  <c:v>193</c:v>
-                </c:pt>
-                <c:pt idx="285">
-                  <c:v>194</c:v>
-                </c:pt>
-                <c:pt idx="286">
-                  <c:v>185</c:v>
-                </c:pt>
-                <c:pt idx="287">
-                  <c:v>201</c:v>
-                </c:pt>
-                <c:pt idx="288">
-                  <c:v>190</c:v>
-                </c:pt>
-                <c:pt idx="289">
-                  <c:v>201</c:v>
-                </c:pt>
-                <c:pt idx="290">
-                  <c:v>197</c:v>
-                </c:pt>
-                <c:pt idx="291">
-                  <c:v>181</c:v>
-                </c:pt>
-                <c:pt idx="292">
-                  <c:v>190</c:v>
-                </c:pt>
-                <c:pt idx="293">
-                  <c:v>195</c:v>
-                </c:pt>
-                <c:pt idx="294">
-                  <c:v>181</c:v>
-                </c:pt>
-                <c:pt idx="295">
-                  <c:v>191</c:v>
-                </c:pt>
-                <c:pt idx="296">
-                  <c:v>187</c:v>
-                </c:pt>
-                <c:pt idx="297">
-                  <c:v>193</c:v>
-                </c:pt>
-                <c:pt idx="298">
-                  <c:v>195</c:v>
-                </c:pt>
-                <c:pt idx="299">
-                  <c:v>197</c:v>
-                </c:pt>
-                <c:pt idx="300">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="301">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="302">
-                  <c:v>191</c:v>
-                </c:pt>
-                <c:pt idx="303">
-                  <c:v>205</c:v>
-                </c:pt>
-                <c:pt idx="304">
-                  <c:v>187</c:v>
-                </c:pt>
-                <c:pt idx="305">
-                  <c:v>201</c:v>
-                </c:pt>
-                <c:pt idx="306">
-                  <c:v>187</c:v>
-                </c:pt>
-                <c:pt idx="307">
-                  <c:v>203</c:v>
-                </c:pt>
-                <c:pt idx="308">
-                  <c:v>195</c:v>
-                </c:pt>
-                <c:pt idx="309">
-                  <c:v>199</c:v>
-                </c:pt>
-                <c:pt idx="310">
-                  <c:v>195</c:v>
-                </c:pt>
-                <c:pt idx="311">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="312">
-                  <c:v>192</c:v>
-                </c:pt>
-                <c:pt idx="313">
-                  <c:v>205</c:v>
-                </c:pt>
-                <c:pt idx="314">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="315">
-                  <c:v>187</c:v>
-                </c:pt>
-                <c:pt idx="316">
-                  <c:v>196</c:v>
-                </c:pt>
-                <c:pt idx="317">
-                  <c:v>196</c:v>
-                </c:pt>
-                <c:pt idx="318">
-                  <c:v>196</c:v>
-                </c:pt>
-                <c:pt idx="319">
-                  <c:v>201</c:v>
-                </c:pt>
-                <c:pt idx="320">
-                  <c:v>190</c:v>
-                </c:pt>
-                <c:pt idx="321">
-                  <c:v>212</c:v>
-                </c:pt>
-                <c:pt idx="322">
-                  <c:v>187</c:v>
-                </c:pt>
-                <c:pt idx="323">
-                  <c:v>198</c:v>
-                </c:pt>
-                <c:pt idx="324">
-                  <c:v>199</c:v>
-                </c:pt>
-                <c:pt idx="325">
-                  <c:v>201</c:v>
-                </c:pt>
-                <c:pt idx="326">
-                  <c:v>193</c:v>
-                </c:pt>
-                <c:pt idx="327">
-                  <c:v>203</c:v>
-                </c:pt>
-                <c:pt idx="328">
-                  <c:v>187</c:v>
-                </c:pt>
-                <c:pt idx="329">
-                  <c:v>197</c:v>
-                </c:pt>
-                <c:pt idx="330">
-                  <c:v>191</c:v>
-                </c:pt>
-                <c:pt idx="331">
-                  <c:v>203</c:v>
-                </c:pt>
-                <c:pt idx="332">
-                  <c:v>202</c:v>
-                </c:pt>
-                <c:pt idx="333">
-                  <c:v>194</c:v>
-                </c:pt>
-                <c:pt idx="334">
-                  <c:v>206</c:v>
-                </c:pt>
-                <c:pt idx="335">
-                  <c:v>189</c:v>
-                </c:pt>
-                <c:pt idx="336">
-                  <c:v>195</c:v>
-                </c:pt>
-                <c:pt idx="337">
-                  <c:v>207</c:v>
-                </c:pt>
-                <c:pt idx="338">
-                  <c:v>202</c:v>
-                </c:pt>
-                <c:pt idx="339">
-                  <c:v>193</c:v>
-                </c:pt>
-                <c:pt idx="340">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="341">
-                  <c:v>198</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>kf_excel_penglings!$G$2:$G$345</c:f>
+              <c:f>kf_excel_penglings!$G$2:$G$153</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="342"/>
+                <c:ptCount val="151"/>
                 <c:pt idx="0">
                   <c:v>3750</c:v>
                 </c:pt>
@@ -2166,579 +1591,6 @@
                 </c:pt>
                 <c:pt idx="150">
                   <c:v>4000</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>4500</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>5700</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>4450</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>5700</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>5400</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>4550</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>4800</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>5200</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>4400</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>5150</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>4650</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>5550</c:v>
-                </c:pt>
-                <c:pt idx="163">
-                  <c:v>4650</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>5850</c:v>
-                </c:pt>
-                <c:pt idx="165">
-                  <c:v>4200</c:v>
-                </c:pt>
-                <c:pt idx="166">
-                  <c:v>5850</c:v>
-                </c:pt>
-                <c:pt idx="167">
-                  <c:v>4150</c:v>
-                </c:pt>
-                <c:pt idx="168">
-                  <c:v>6300</c:v>
-                </c:pt>
-                <c:pt idx="169">
-                  <c:v>4800</c:v>
-                </c:pt>
-                <c:pt idx="170">
-                  <c:v>5350</c:v>
-                </c:pt>
-                <c:pt idx="171">
-                  <c:v>5700</c:v>
-                </c:pt>
-                <c:pt idx="172">
-                  <c:v>5000</c:v>
-                </c:pt>
-                <c:pt idx="173">
-                  <c:v>4400</c:v>
-                </c:pt>
-                <c:pt idx="174">
-                  <c:v>5050</c:v>
-                </c:pt>
-                <c:pt idx="175">
-                  <c:v>5000</c:v>
-                </c:pt>
-                <c:pt idx="176">
-                  <c:v>5100</c:v>
-                </c:pt>
-                <c:pt idx="177">
-                  <c:v>4100</c:v>
-                </c:pt>
-                <c:pt idx="178">
-                  <c:v>5650</c:v>
-                </c:pt>
-                <c:pt idx="179">
-                  <c:v>4600</c:v>
-                </c:pt>
-                <c:pt idx="180">
-                  <c:v>5550</c:v>
-                </c:pt>
-                <c:pt idx="181">
-                  <c:v>5250</c:v>
-                </c:pt>
-                <c:pt idx="182">
-                  <c:v>4700</c:v>
-                </c:pt>
-                <c:pt idx="183">
-                  <c:v>5050</c:v>
-                </c:pt>
-                <c:pt idx="184">
-                  <c:v>6050</c:v>
-                </c:pt>
-                <c:pt idx="185">
-                  <c:v>5150</c:v>
-                </c:pt>
-                <c:pt idx="186">
-                  <c:v>5400</c:v>
-                </c:pt>
-                <c:pt idx="187">
-                  <c:v>4950</c:v>
-                </c:pt>
-                <c:pt idx="188">
-                  <c:v>5250</c:v>
-                </c:pt>
-                <c:pt idx="189">
-                  <c:v>4350</c:v>
-                </c:pt>
-                <c:pt idx="190">
-                  <c:v>5350</c:v>
-                </c:pt>
-                <c:pt idx="191">
-                  <c:v>3950</c:v>
-                </c:pt>
-                <c:pt idx="192">
-                  <c:v>5700</c:v>
-                </c:pt>
-                <c:pt idx="193">
-                  <c:v>4300</c:v>
-                </c:pt>
-                <c:pt idx="194">
-                  <c:v>4750</c:v>
-                </c:pt>
-                <c:pt idx="195">
-                  <c:v>5550</c:v>
-                </c:pt>
-                <c:pt idx="196">
-                  <c:v>4900</c:v>
-                </c:pt>
-                <c:pt idx="197">
-                  <c:v>4200</c:v>
-                </c:pt>
-                <c:pt idx="198">
-                  <c:v>5400</c:v>
-                </c:pt>
-                <c:pt idx="199">
-                  <c:v>5100</c:v>
-                </c:pt>
-                <c:pt idx="200">
-                  <c:v>5300</c:v>
-                </c:pt>
-                <c:pt idx="201">
-                  <c:v>4850</c:v>
-                </c:pt>
-                <c:pt idx="202">
-                  <c:v>5300</c:v>
-                </c:pt>
-                <c:pt idx="203">
-                  <c:v>4400</c:v>
-                </c:pt>
-                <c:pt idx="204">
-                  <c:v>5000</c:v>
-                </c:pt>
-                <c:pt idx="205">
-                  <c:v>4900</c:v>
-                </c:pt>
-                <c:pt idx="206">
-                  <c:v>5050</c:v>
-                </c:pt>
-                <c:pt idx="207">
-                  <c:v>4300</c:v>
-                </c:pt>
-                <c:pt idx="208">
-                  <c:v>5000</c:v>
-                </c:pt>
-                <c:pt idx="209">
-                  <c:v>4450</c:v>
-                </c:pt>
-                <c:pt idx="210">
-                  <c:v>5550</c:v>
-                </c:pt>
-                <c:pt idx="211">
-                  <c:v>4200</c:v>
-                </c:pt>
-                <c:pt idx="212">
-                  <c:v>5300</c:v>
-                </c:pt>
-                <c:pt idx="213">
-                  <c:v>4400</c:v>
-                </c:pt>
-                <c:pt idx="214">
-                  <c:v>5650</c:v>
-                </c:pt>
-                <c:pt idx="215">
-                  <c:v>4700</c:v>
-                </c:pt>
-                <c:pt idx="216">
-                  <c:v>5700</c:v>
-                </c:pt>
-                <c:pt idx="217">
-                  <c:v>4650</c:v>
-                </c:pt>
-                <c:pt idx="218">
-                  <c:v>5800</c:v>
-                </c:pt>
-                <c:pt idx="219">
-                  <c:v>4700</c:v>
-                </c:pt>
-                <c:pt idx="220">
-                  <c:v>5550</c:v>
-                </c:pt>
-                <c:pt idx="221">
-                  <c:v>4750</c:v>
-                </c:pt>
-                <c:pt idx="222">
-                  <c:v>5000</c:v>
-                </c:pt>
-                <c:pt idx="223">
-                  <c:v>5100</c:v>
-                </c:pt>
-                <c:pt idx="224">
-                  <c:v>5200</c:v>
-                </c:pt>
-                <c:pt idx="225">
-                  <c:v>4700</c:v>
-                </c:pt>
-                <c:pt idx="226">
-                  <c:v>5800</c:v>
-                </c:pt>
-                <c:pt idx="227">
-                  <c:v>4600</c:v>
-                </c:pt>
-                <c:pt idx="228">
-                  <c:v>6000</c:v>
-                </c:pt>
-                <c:pt idx="229">
-                  <c:v>4750</c:v>
-                </c:pt>
-                <c:pt idx="230">
-                  <c:v>5950</c:v>
-                </c:pt>
-                <c:pt idx="231">
-                  <c:v>4625</c:v>
-                </c:pt>
-                <c:pt idx="232">
-                  <c:v>5450</c:v>
-                </c:pt>
-                <c:pt idx="233">
-                  <c:v>4725</c:v>
-                </c:pt>
-                <c:pt idx="234">
-                  <c:v>5350</c:v>
-                </c:pt>
-                <c:pt idx="235">
-                  <c:v>4750</c:v>
-                </c:pt>
-                <c:pt idx="236">
-                  <c:v>5600</c:v>
-                </c:pt>
-                <c:pt idx="237">
-                  <c:v>4600</c:v>
-                </c:pt>
-                <c:pt idx="238">
-                  <c:v>5300</c:v>
-                </c:pt>
-                <c:pt idx="239">
-                  <c:v>4875</c:v>
-                </c:pt>
-                <c:pt idx="240">
-                  <c:v>5550</c:v>
-                </c:pt>
-                <c:pt idx="241">
-                  <c:v>4950</c:v>
-                </c:pt>
-                <c:pt idx="242">
-                  <c:v>5400</c:v>
-                </c:pt>
-                <c:pt idx="243">
-                  <c:v>4750</c:v>
-                </c:pt>
-                <c:pt idx="244">
-                  <c:v>5650</c:v>
-                </c:pt>
-                <c:pt idx="245">
-                  <c:v>4850</c:v>
-                </c:pt>
-                <c:pt idx="246">
-                  <c:v>5200</c:v>
-                </c:pt>
-                <c:pt idx="247">
-                  <c:v>4925</c:v>
-                </c:pt>
-                <c:pt idx="248">
-                  <c:v>4875</c:v>
-                </c:pt>
-                <c:pt idx="249">
-                  <c:v>4625</c:v>
-                </c:pt>
-                <c:pt idx="250">
-                  <c:v>5250</c:v>
-                </c:pt>
-                <c:pt idx="251">
-                  <c:v>4850</c:v>
-                </c:pt>
-                <c:pt idx="252">
-                  <c:v>5600</c:v>
-                </c:pt>
-                <c:pt idx="253">
-                  <c:v>4975</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v>5500</c:v>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v>4725</c:v>
-                </c:pt>
-                <c:pt idx="256">
-                  <c:v>5500</c:v>
-                </c:pt>
-                <c:pt idx="257">
-                  <c:v>4700</c:v>
-                </c:pt>
-                <c:pt idx="258">
-                  <c:v>5500</c:v>
-                </c:pt>
-                <c:pt idx="259">
-                  <c:v>4575</c:v>
-                </c:pt>
-                <c:pt idx="260">
-                  <c:v>5500</c:v>
-                </c:pt>
-                <c:pt idx="261">
-                  <c:v>5000</c:v>
-                </c:pt>
-                <c:pt idx="262">
-                  <c:v>5950</c:v>
-                </c:pt>
-                <c:pt idx="263">
-                  <c:v>4650</c:v>
-                </c:pt>
-                <c:pt idx="264">
-                  <c:v>5500</c:v>
-                </c:pt>
-                <c:pt idx="265">
-                  <c:v>4375</c:v>
-                </c:pt>
-                <c:pt idx="266">
-                  <c:v>5850</c:v>
-                </c:pt>
-                <c:pt idx="267">
-                  <c:v>4875</c:v>
-                </c:pt>
-                <c:pt idx="268">
-                  <c:v>6000</c:v>
-                </c:pt>
-                <c:pt idx="269">
-                  <c:v>4925</c:v>
-                </c:pt>
-                <c:pt idx="270">
-                  <c:v>4850</c:v>
-                </c:pt>
-                <c:pt idx="271">
-                  <c:v>5750</c:v>
-                </c:pt>
-                <c:pt idx="272">
-                  <c:v>5200</c:v>
-                </c:pt>
-                <c:pt idx="273">
-                  <c:v>5400</c:v>
-                </c:pt>
-                <c:pt idx="274">
-                  <c:v>3500</c:v>
-                </c:pt>
-                <c:pt idx="275">
-                  <c:v>3900</c:v>
-                </c:pt>
-                <c:pt idx="276">
-                  <c:v>3650</c:v>
-                </c:pt>
-                <c:pt idx="277">
-                  <c:v>3525</c:v>
-                </c:pt>
-                <c:pt idx="278">
-                  <c:v>3725</c:v>
-                </c:pt>
-                <c:pt idx="279">
-                  <c:v>3950</c:v>
-                </c:pt>
-                <c:pt idx="280">
-                  <c:v>3250</c:v>
-                </c:pt>
-                <c:pt idx="281">
-                  <c:v>3750</c:v>
-                </c:pt>
-                <c:pt idx="282">
-                  <c:v>4150</c:v>
-                </c:pt>
-                <c:pt idx="283">
-                  <c:v>3700</c:v>
-                </c:pt>
-                <c:pt idx="284">
-                  <c:v>3800</c:v>
-                </c:pt>
-                <c:pt idx="285">
-                  <c:v>3775</c:v>
-                </c:pt>
-                <c:pt idx="286">
-                  <c:v>3700</c:v>
-                </c:pt>
-                <c:pt idx="287">
-                  <c:v>4050</c:v>
-                </c:pt>
-                <c:pt idx="288">
-                  <c:v>3575</c:v>
-                </c:pt>
-                <c:pt idx="289">
-                  <c:v>4050</c:v>
-                </c:pt>
-                <c:pt idx="290">
-                  <c:v>3300</c:v>
-                </c:pt>
-                <c:pt idx="291">
-                  <c:v>3700</c:v>
-                </c:pt>
-                <c:pt idx="292">
-                  <c:v>3450</c:v>
-                </c:pt>
-                <c:pt idx="293">
-                  <c:v>4400</c:v>
-                </c:pt>
-                <c:pt idx="294">
-                  <c:v>3600</c:v>
-                </c:pt>
-                <c:pt idx="295">
-                  <c:v>3400</c:v>
-                </c:pt>
-                <c:pt idx="296">
-                  <c:v>2900</c:v>
-                </c:pt>
-                <c:pt idx="297">
-                  <c:v>3800</c:v>
-                </c:pt>
-                <c:pt idx="298">
-                  <c:v>3300</c:v>
-                </c:pt>
-                <c:pt idx="299">
-                  <c:v>4150</c:v>
-                </c:pt>
-                <c:pt idx="300">
-                  <c:v>3400</c:v>
-                </c:pt>
-                <c:pt idx="301">
-                  <c:v>3800</c:v>
-                </c:pt>
-                <c:pt idx="302">
-                  <c:v>3700</c:v>
-                </c:pt>
-                <c:pt idx="303">
-                  <c:v>4550</c:v>
-                </c:pt>
-                <c:pt idx="304">
-                  <c:v>3200</c:v>
-                </c:pt>
-                <c:pt idx="305">
-                  <c:v>4300</c:v>
-                </c:pt>
-                <c:pt idx="306">
-                  <c:v>3350</c:v>
-                </c:pt>
-                <c:pt idx="307">
-                  <c:v>4100</c:v>
-                </c:pt>
-                <c:pt idx="308">
-                  <c:v>3600</c:v>
-                </c:pt>
-                <c:pt idx="309">
-                  <c:v>3900</c:v>
-                </c:pt>
-                <c:pt idx="310">
-                  <c:v>3850</c:v>
-                </c:pt>
-                <c:pt idx="311">
-                  <c:v>4800</c:v>
-                </c:pt>
-                <c:pt idx="312">
-                  <c:v>2700</c:v>
-                </c:pt>
-                <c:pt idx="313">
-                  <c:v>4500</c:v>
-                </c:pt>
-                <c:pt idx="314">
-                  <c:v>3950</c:v>
-                </c:pt>
-                <c:pt idx="315">
-                  <c:v>3650</c:v>
-                </c:pt>
-                <c:pt idx="316">
-                  <c:v>3550</c:v>
-                </c:pt>
-                <c:pt idx="317">
-                  <c:v>3500</c:v>
-                </c:pt>
-                <c:pt idx="318">
-                  <c:v>3675</c:v>
-                </c:pt>
-                <c:pt idx="319">
-                  <c:v>4450</c:v>
-                </c:pt>
-                <c:pt idx="320">
-                  <c:v>3400</c:v>
-                </c:pt>
-                <c:pt idx="321">
-                  <c:v>4300</c:v>
-                </c:pt>
-                <c:pt idx="322">
-                  <c:v>3250</c:v>
-                </c:pt>
-                <c:pt idx="323">
-                  <c:v>3675</c:v>
-                </c:pt>
-                <c:pt idx="324">
-                  <c:v>3325</c:v>
-                </c:pt>
-                <c:pt idx="325">
-                  <c:v>3950</c:v>
-                </c:pt>
-                <c:pt idx="326">
-                  <c:v>3600</c:v>
-                </c:pt>
-                <c:pt idx="327">
-                  <c:v>4050</c:v>
-                </c:pt>
-                <c:pt idx="328">
-                  <c:v>3350</c:v>
-                </c:pt>
-                <c:pt idx="329">
-                  <c:v>3450</c:v>
-                </c:pt>
-                <c:pt idx="330">
-                  <c:v>3250</c:v>
-                </c:pt>
-                <c:pt idx="331">
-                  <c:v>4050</c:v>
-                </c:pt>
-                <c:pt idx="332">
-                  <c:v>3800</c:v>
-                </c:pt>
-                <c:pt idx="333">
-                  <c:v>3525</c:v>
-                </c:pt>
-                <c:pt idx="334">
-                  <c:v>3950</c:v>
-                </c:pt>
-                <c:pt idx="335">
-                  <c:v>3650</c:v>
-                </c:pt>
-                <c:pt idx="336">
-                  <c:v>3650</c:v>
-                </c:pt>
-                <c:pt idx="337">
-                  <c:v>4000</c:v>
-                </c:pt>
-                <c:pt idx="338">
-                  <c:v>3400</c:v>
-                </c:pt>
-                <c:pt idx="339">
-                  <c:v>3775</c:v>
-                </c:pt>
-                <c:pt idx="340">
-                  <c:v>4100</c:v>
-                </c:pt>
-                <c:pt idx="341">
-                  <c:v>3775</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2746,7 +1598,1259 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-15A1-46EF-AEF3-1627206F7442}"/>
+              <c16:uniqueId val="{00000000-FD45-4180-B1B8-25EEFD84FE6E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Gentoo</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="21C1A6">
+                  <a:alpha val="70000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>kf_excel_penglings!$F$154:$F$277</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="123"/>
+                <c:pt idx="0">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>221</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>222</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>222</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>207</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>222</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>221</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>231</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>229</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>223</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>221</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>221</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>223</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>221</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>222</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>203</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>229</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>222</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>222</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>213</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>kf_excel_penglings!$G$154:$G$277</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="123"/>
+                <c:pt idx="0">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5700</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4450</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5700</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4550</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4800</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4400</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5150</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4650</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5550</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4650</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5850</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4200</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5850</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4150</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6300</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4800</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5350</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5700</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4400</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5050</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5100</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5650</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4600</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5550</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5250</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4700</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5050</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6050</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5150</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5400</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4950</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5250</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4350</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>5350</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3950</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>5700</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4750</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>5550</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4900</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4200</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>5400</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>5100</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>5300</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4850</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>5300</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4400</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4900</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>5050</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>4450</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>5550</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>4200</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>5300</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>4400</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>5650</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>4700</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>5700</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>4650</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>5800</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>4700</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>5550</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>4750</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>5100</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>5200</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>4700</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>5800</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>4600</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>4750</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>5950</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>4625</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>5450</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>4725</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>5350</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>4750</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>5600</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>4600</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>5300</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>4875</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>5550</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>4950</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>5400</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>4750</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>5650</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>4850</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>5200</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>4925</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>4875</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>4625</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>5250</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>4850</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>5600</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>4975</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>5500</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>4725</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>5500</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>4700</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>5500</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>4575</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>5500</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>5950</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>4650</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>5500</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>4375</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>5850</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>4875</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>4925</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>4850</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>5750</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>5200</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>5400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FD45-4180-B1B8-25EEFD84FE6E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Chinstrap</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="D256C3">
+                  <a:alpha val="70000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>kf_excel_penglings!$F$278:$F$345</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="68"/>
+                <c:pt idx="0">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>188</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>181</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>181</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>203</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>199</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>199</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>203</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>203</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>202</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>206</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>189</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>207</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>202</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>198</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>kf_excel_penglings!$G$278:$G$345</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="68"/>
+                <c:pt idx="0">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3900</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3650</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3525</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3725</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3950</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3250</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3750</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4150</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3700</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3800</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3775</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3700</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4050</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3575</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4050</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3300</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3700</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3450</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4400</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3600</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3400</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2900</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3800</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3300</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4150</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3400</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3800</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3700</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4550</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3200</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3350</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3600</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3900</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3850</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4800</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2700</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3950</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>3650</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3550</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3675</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4450</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>3400</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3250</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>3675</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>3325</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>3950</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>3600</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>4050</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>3350</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>3450</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3250</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>4050</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3800</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>3525</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>3950</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>3650</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>3650</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>3400</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>3775</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>3775</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FD45-4180-B1B8-25EEFD84FE6E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3016,10 +3120,7 @@
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="accent1"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -3604,15 +3705,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>452719</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>170330</xdr:rowOff>
+      <xdr:colOff>596155</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>80683</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>147919</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>44824</xdr:rowOff>
+      <xdr:colOff>291355</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4037,8 +4138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA2D589A-6F7E-4317-8AE2-C5DD35030204}">
   <dimension ref="A1:I345"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added screenshots of the recreated visualizations and modified the README (also added a legend for Excel implementation)
</commit_message>
<xml_diff>
--- a/all_visualizations/kf_excel_penglings.csv.xlsx
+++ b/all_visualizations/kf_excel_penglings.csv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klaud\WebstormProjects\klaudio-fusha-a2-datavis-5ways\a2-DataVis-5ways\all_visualizations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4009C333-5ECC-43EB-931B-82C8FF0B3C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032DEE74-C74D-402B-A587-6C141488F088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{298BFD60-299E-47A5-8AF2-E192D2EEC218}"/>
   </bookViews>
@@ -4172,6 +4172,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>

</xml_diff>